<commit_message>
Update Dataset S1 with new version
</commit_message>
<xml_diff>
--- a/data/DatasetS1.xlsx
+++ b/data/DatasetS1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\Postdoc1\supplementary_information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\Postdoc1\ECCO-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6029DE6E-1BB1-421E-8BDA-6947080FB040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED5785-7802-4AF0-8F3C-093F4160804A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E7BEDB3-EB18-443B-A872-1994BB58BA21}"/>
   </bookViews>
@@ -335,9 +335,6 @@
     <t>Region</t>
   </si>
   <si>
-    <t>This Excel file compiles information on sociopolitical complexity over time, based on the first ans second principal component (PC1, and PC2) from Turchin et al. 2017, which summarizes 51 variables related to the evolution of social complexity in 30 natural geographic regions during the last 10,000 years. For each region, we calculated the area under the curve (AUC) of PC1 and PC2 values over time to represent the cumulative trajectory of sociopolitical complexity. Each HGDP population was matched with the corresponding or nearest region from Turchin et al. (2017).</t>
-  </si>
-  <si>
     <t>Seshat population</t>
   </si>
   <si>
@@ -388,6 +385,9 @@
       </rPr>
       <t>Area under the curve (AUC) of sociopolitical complexity trajectories across the 54 populations of the Human Genome Diversity Project (HGDP)</t>
     </r>
+  </si>
+  <si>
+    <t>This Excel file compiles information on sociopolitical complexity over time, based on the first and second principal component (PC1, and PC2) from Turchin et al. 2017, which summarizes 51 variables related to the evolution of social complexity in 30 natural geographic regions during the last 10,000 years. For each region, we calculated the area under the curve (AUC) of PC1 and PC2 values over time to represent the cumulative trajectory of sociopolitical complexity. Each HGDP population was matched with the corresponding or nearest region from Turchin et al. (2017).</t>
   </si>
 </sst>
 </file>
@@ -874,18 +874,18 @@
   <sheetData>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B3" s="25"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="20"/>
     </row>
@@ -898,7 +898,7 @@
         <v>98</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -914,7 +914,7 @@
         <v>78</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -922,36 +922,36 @@
         <v>79</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -985,7 +985,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" s="26"/>
     </row>
@@ -1003,7 +1003,7 @@
         <v>79</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>0</v>

</xml_diff>